<commit_message>
Update for adding Ltdexp Scenarios and Routes
</commit_message>
<xml_diff>
--- a/Jibei_Railway/Structures/StationName/編集用.xlsx
+++ b/Jibei_Railway/Structures/StationName/編集用.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\33752\Documents\BveTs\Scenarios_Work\Jibei_Railway\Structures\StationName\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF69D85-CCB9-4EF5-B4C3-124EB2C654D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38D15FD-240B-4E41-A1DB-79B869EF91E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{DE6CD4EC-68BC-496D-9896-0F41ECF51F3E}"/>
+    <workbookView xWindow="3200" yWindow="1990" windowWidth="19200" windowHeight="9970" xr2:uid="{DE6CD4EC-68BC-496D-9896-0F41ECF51F3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,56 +81,122 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>新大学城</t>
+    <r>
+      <t xml:space="preserve">For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Lifujing &amp; Jibei Airport</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="9"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>济</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="9"/>
+        <rFont val="小塚ゴシック Pr6N R"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>北本</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="9"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>线</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="9"/>
+        <rFont val="小塚ゴシック Pr6N R"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>　Jibei Main</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="小塚ゴシック Pr6N R"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve"> L</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="9"/>
+        <rFont val="小塚ゴシック Pr6N R"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ine</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>カナヤマ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>セン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>王符河</t>
     <rPh sb="0" eb="3">
       <t>ゴジョウガワ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>新大学城</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Xin Da Xue Cheng</t>
+    <t>Wang Fu He</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <r>
-      <t>[</t>
+      <t>[JM-2</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="20"/>
-        <color indexed="9"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>JM</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <color indexed="9"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="小塚ゴシック Pr6N B"/>
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <color indexed="9"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>31</t>
+      <t>8</t>
     </r>
     <r>
       <rPr>
@@ -146,60 +212,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color indexed="9"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>济北本线</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color indexed="9"/>
-        <rFont val="小塚ゴシック Pr6N R"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>　Jibei</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color indexed="9"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color indexed="9"/>
-        <rFont val="小塚ゴシック Pr6N R"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>Main line</t>
-    </r>
-    <rPh sb="0" eb="2">
-      <t>カナヤマ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>セン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>　Ziweijiedao</t>
+    <t>王符河</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -210,12 +223,34 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color indexed="9"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="小塚ゴシック Pr6N R"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>新</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="等线"/>
-        <family val="3"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>紫薇街道</t>
+      <t>赵营</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="小塚ゴシック Pr6N R"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>子</t>
     </r>
     <r>
       <rPr>
@@ -226,40 +261,18 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t>[</t>
+      <t>[JM-</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="14"/>
-        <color indexed="9"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>JM</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color indexed="9"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="小塚ゴシック Pr6N R"/>
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color indexed="9"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>30</t>
+      <t>29</t>
     </r>
     <r>
       <rPr>
@@ -276,13 +289,30 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Xinzhaoyingzi</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="14"/>
         <color rgb="FFFFFFFF"/>
-        <rFont val="等线"/>
+        <rFont val="小塚ゴシック Pr6N R"/>
         <family val="2"/>
-        <charset val="134"/>
+        <charset val="128"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -295,18 +325,18 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t>[</t>
+      <t>[JM-</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="14"/>
-        <color indexed="9"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="小塚ゴシック Pr6N R"/>
+        <family val="2"/>
+        <charset val="128"/>
       </rPr>
-      <t>JM</t>
+      <t>27</t>
     </r>
     <r>
       <rPr>
@@ -317,62 +347,23 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t>-3</t>
+      <t>][JF-01]</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="14"/>
         <color rgb="FFFFFFFF"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color indexed="9"/>
         <rFont val="小塚ゴシック Pr6N R"/>
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t>]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>世博园</t>
+      <t>李府井</t>
     </r>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve"> Shiboyuan</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">For </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Lifujing &amp; Jibei Airport</t>
-    </r>
+    <t xml:space="preserve"> Lifujing </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -380,7 +371,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -420,13 +411,6 @@
       <name val="小塚ゴシック Pr6N R"/>
       <family val="2"/>
       <charset val="128"/>
-    </font>
-    <font>
-      <sz val="48"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="黑体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="60"/>
@@ -511,14 +495,6 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
-      <color indexed="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
       <sz val="16"/>
       <color indexed="9"/>
       <name val="小塚ゴシック Pr6N R"/>
@@ -543,27 +519,11 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color indexed="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color indexed="9"/>
       <name val="小塚ゴシック Pr6N R"/>
       <family val="2"/>
       <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color indexed="9"/>
-      <name val="小塚ゴシック Pr6N R"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -612,6 +572,46 @@
       <name val="黑体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="小塚ゴシック Pr6N R"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="48"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="黑体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="小塚ゴシック Pr6N R"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="小塚ゴシック Pr6N B"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="7">
@@ -746,7 +746,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -768,107 +768,110 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1104,6 +1107,372 @@
         <a:xfrm>
           <a:off x="5124174" y="4566478"/>
           <a:ext cx="4958522" cy="1244239"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>369957</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>60146</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="图片 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF4950F6-69F1-A280-25C2-4588636597A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="6057348"/>
+          <a:ext cx="4853609" cy="1219711"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>456544</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>77304</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="图片 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB6AD514-FA7B-0021-97D3-7B903F826F35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5124174" y="6057348"/>
+          <a:ext cx="4929153" cy="1236869"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>364435</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>58760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94AC0741-73A5-4E05-4196-556A0A3349CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="7382566"/>
+          <a:ext cx="4848087" cy="1218324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>430695</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>70818</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A240772-FBC5-E8ED-C11C-D022EBF484DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5124174" y="7382565"/>
+          <a:ext cx="4903304" cy="1230383"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>372314</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>60739</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="图片 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16FFF03B-DFF9-3F03-4F5A-796557E3BF3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="8707783"/>
+          <a:ext cx="4855966" cy="1220304"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>419652</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>68047</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="图片 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B593820-2D26-AE14-17A9-16EB84210AAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5124174" y="8707783"/>
+          <a:ext cx="4892261" cy="1227612"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1979,8 +2348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C45CCD5-3E6B-42CC-BACB-505396A89B7C}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13"/>
@@ -2012,14 +2381,14 @@
       <c r="D2" s="25" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>4</v>
+      <c r="E2" s="40" t="s">
+        <v>6</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -2030,17 +2399,17 @@
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="25"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="12.75" customHeight="1">
@@ -2048,12 +2417,12 @@
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="25"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -2061,7 +2430,7 @@
     </row>
     <row r="5" spans="1:14" ht="20.25" customHeight="1">
       <c r="A5" s="23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -2079,7 +2448,7 @@
     </row>
     <row r="6" spans="1:14" ht="20.25" customHeight="1">
       <c r="A6" s="23" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
@@ -2096,22 +2465,22 @@
       <c r="N6" s="24"/>
     </row>
     <row r="7" spans="1:14" ht="20.25" customHeight="1">
-      <c r="A7" s="21" t="s">
-        <v>8</v>
+      <c r="A7" s="22" t="s">
+        <v>5</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A8" s="27" t="s">
@@ -2128,7 +2497,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M8" s="26"/>
       <c r="N8" s="26"/>
@@ -2150,11 +2519,11 @@
       <c r="N9" s="26"/>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="19" t="s">
-        <v>9</v>
+      <c r="A10" s="41" t="s">
+        <v>11</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2163,11 +2532,11 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="20" t="s">
-        <v>12</v>
+      <c r="L10" s="21" t="s">
+        <v>13</v>
       </c>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2193,7 +2562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF78DA62-F086-4E94-AE36-F8701B11A0B0}">
   <dimension ref="A15:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X48" sqref="X48"/>
     </sheetView>
   </sheetViews>
@@ -2225,10 +2594,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="28"/>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="34"/>
+      <c r="D15" s="36"/>
       <c r="E15" s="9"/>
       <c r="F15" s="29" t="s">
         <v>2</v>
@@ -2237,10 +2606,10 @@
       <c r="H15" s="29"/>
       <c r="I15" s="30"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="39" t="s">
+      <c r="K15" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="L15" s="39"/>
+      <c r="L15" s="34"/>
       <c r="M15" s="11"/>
       <c r="N15" s="29" t="s">
         <v>2</v>
@@ -2249,10 +2618,10 @@
       <c r="P15" s="29"/>
       <c r="Q15" s="30"/>
       <c r="R15" s="9"/>
-      <c r="S15" s="35" t="s">
+      <c r="S15" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="T15" s="35"/>
+      <c r="T15" s="37"/>
       <c r="U15" s="28">
         <v>3</v>
       </c>
@@ -2261,37 +2630,37 @@
     <row r="16" spans="1:22" ht="13.5" customHeight="1">
       <c r="A16" s="28"/>
       <c r="B16" s="28"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
       <c r="E16" s="9"/>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
       <c r="H16" s="29"/>
       <c r="I16" s="30"/>
       <c r="J16" s="12"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
       <c r="M16" s="13"/>
       <c r="N16" s="29"/>
       <c r="O16" s="29"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="30"/>
       <c r="R16" s="9"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
       <c r="U16" s="28"/>
       <c r="V16" s="28"/>
     </row>
     <row r="17" spans="1:22" ht="13.5" customHeight="1">
       <c r="A17" s="28"/>
       <c r="B17" s="28"/>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="37"/>
+      <c r="D17" s="39"/>
       <c r="E17" s="9"/>
       <c r="F17" s="31" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="32"/>
@@ -2301,16 +2670,16 @@
       <c r="L17" s="16"/>
       <c r="M17" s="13"/>
       <c r="N17" s="31" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="O17" s="32"/>
       <c r="P17" s="32"/>
       <c r="Q17" s="33"/>
       <c r="R17" s="9"/>
-      <c r="S17" s="36" t="s">
+      <c r="S17" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="T17" s="36"/>
+      <c r="T17" s="38"/>
       <c r="U17" s="28"/>
       <c r="V17" s="28"/>
     </row>
@@ -2333,8 +2702,8 @@
       <c r="P18" s="32"/>
       <c r="Q18" s="33"/>
       <c r="R18" s="9"/>
-      <c r="S18" s="38"/>
-      <c r="T18" s="38"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
       <c r="U18" s="28"/>
       <c r="V18" s="28"/>
     </row>

</xml_diff>